<commit_message>
adds sort by name, impove sorting code
</commit_message>
<xml_diff>
--- a/CW2-member-contribution.xlsx
+++ b/CW2-member-contribution.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21231"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A6FD026-B3FD-4CBD-A448-F11C4ECBE3DD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43B8ECFD-4753-45AB-B948-0D90B68E5E85}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Group Size 3" sheetId="1" r:id="rId1"/>
@@ -16,6 +16,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -547,8 +548,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -636,7 +637,7 @@
         <v>3</v>
       </c>
       <c r="C8" s="10">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D8" s="11">
         <v>1</v>
@@ -661,7 +662,7 @@
         <v>3</v>
       </c>
       <c r="C9" s="10">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D9" s="11">
         <v>1</v>
@@ -689,10 +690,10 @@
         <v>0</v>
       </c>
       <c r="D10" s="11">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="E10" s="11">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="F10" s="11">
         <v>0</v>
@@ -734,7 +735,7 @@
         <v>3</v>
       </c>
       <c r="C12" s="10">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D12" s="11">
         <v>1</v>
@@ -758,7 +759,7 @@
         <v>3</v>
       </c>
       <c r="C13" s="10">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D13" s="11">
         <v>1</v>
@@ -830,7 +831,7 @@
         <v>3</v>
       </c>
       <c r="C16" s="10">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D16" s="11">
         <v>0.5</v>
@@ -854,7 +855,7 @@
         <v>3</v>
       </c>
       <c r="C17" s="10">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D17" s="11">
         <v>0</v>
@@ -880,7 +881,7 @@
       </c>
       <c r="C18" s="5">
         <f>SUM(C8:C17)</f>
-        <v>18</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
@@ -891,11 +892,11 @@
       <c r="C19" s="6"/>
       <c r="D19" s="5">
         <f t="array" ref="D19">SUM(C8:C17*D8:D17)</f>
-        <v>13.5</v>
+        <v>0</v>
       </c>
       <c r="E19" s="5">
         <f t="array" ref="E19">SUM(C8:C17*E8:E17)</f>
-        <v>4.5</v>
+        <v>0</v>
       </c>
       <c r="F19" s="5">
         <f t="array" ref="F19">SUM(C8:C17*F8:F17)</f>
@@ -925,7 +926,7 @@
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" s="2">
         <f>AVERAGE(D19,E19,F19)</f>
-        <v>6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
@@ -940,7 +941,7 @@
       </c>
       <c r="B28" s="7">
         <f>IF(D19=0,0,C18  + C18 * $A22*(D19-A25)/A25)</f>
-        <v>29.25</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
@@ -950,7 +951,7 @@
       </c>
       <c r="B29" s="7">
         <f>IF(E19=0,0,C18  + C18 * $A22*(E19-A25)/A25)</f>
-        <v>15.75</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
@@ -979,7 +980,7 @@
       </c>
       <c r="B33" s="12">
         <f>IF(B28&gt;B18,B18, B28)</f>
-        <v>29.25</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
@@ -989,7 +990,7 @@
       </c>
       <c r="B34" s="12">
         <f>IF(B29&gt;B18,B18, B29)</f>
-        <v>15.75</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">

</xml_diff>